<commit_message>
Synchro de la bonne présentation
</commit_message>
<xml_diff>
--- a/Gestion/L1 Gestion de risques.xlsx
+++ b/Gestion/L1 Gestion de risques.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederic\Google Drive\Génie Électrique\S5\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg_000\Desktop\Université\S5\Projet\ProjetS5\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="6630" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="6636" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Risques techniques" sheetId="1" r:id="rId1"/>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -342,6 +342,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,27 +669,27 @@
       <selection activeCell="E3" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" style="1" customWidth="1"/>
     <col min="2" max="5" width="10.6640625" style="1"/>
-    <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.46484375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.44140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -706,7 +712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -720,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="1">
-        <f>B3*C3*D3</f>
+        <f t="shared" ref="E3:E12" si="0">B3*C3*D3</f>
         <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -730,7 +736,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -744,7 +750,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <f>B4*C4*D4</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -754,7 +760,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -768,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <f>B5*C5*D5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -778,7 +784,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -792,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="1">
-        <f>B6*C6*D6</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -802,7 +808,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -816,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1">
-        <f>B7*C7*D7</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -826,7 +832,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -840,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1">
-        <f>B8*C8*D8</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -850,7 +856,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -864,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="1">
-        <f>B9*C9*D9</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -874,7 +880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -888,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <f>B10*C10*D10</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -898,7 +904,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -912,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <f>B11*C11*D11</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -922,7 +928,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -936,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="1">
-        <f>B12*C12*D12</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -980,27 +986,27 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" style="1" customWidth="1"/>
     <col min="2" max="5" width="10.6640625" style="1"/>
-    <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.46484375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.44140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="1">
-        <f>B3*C3*D3</f>
+        <f t="shared" ref="E3:E9" si="0">B3*C3*D3</f>
         <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1047,7 +1053,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <f>B4*C4*D4</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1071,7 +1077,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1">
-        <f>B5*C5*D5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1095,7 +1101,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="1">
-        <f>B6*C6*D6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1119,7 +1125,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1">
-        <f>B7*C7*D7</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1143,7 +1149,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1">
-        <f>B8*C8*D8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1167,7 +1173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <f>B9*C9*D9</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1221,43 +1227,43 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.265625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="10.6640625" style="1"/>
-    <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.46484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" style="2"/>
+    <col min="6" max="6" width="44.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.44140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1267,21 +1273,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>5</v>
       </c>
-      <c r="E3" s="1">
-        <f>B3*C3*D3</f>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E12" si="0">B3*C3*D3</f>
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1291,21 +1297,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <f>B4*C4*D4</f>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1315,21 +1321,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <f>B5*C5*D5</f>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1339,21 +1345,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
-        <f>B6*C6*D6</f>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1363,21 +1369,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="1">
-        <f>B7*C7*D7</f>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1387,21 +1393,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1">
-        <f>B8*C8*D8</f>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1411,21 +1417,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1">
-        <f>B9*C9*D9</f>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1435,21 +1441,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1">
-        <f>B10*C10*D10</f>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1459,21 +1465,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="1">
-        <f>B11*C11*D11</f>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1483,21 +1489,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
-        <f>B12*C12*D12</f>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">

</xml_diff>